<commit_message>
Version excel to xml
</commit_message>
<xml_diff>
--- a/io_maping/DS4 connection.xlsx
+++ b/io_maping/DS4 connection.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20235" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1407,7 +1407,7 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K49"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>